<commit_message>
updating deliverables documentes and minifing style.css
</commit_message>
<xml_diff>
--- a/P4/SEO_ANALYSIS.xlsx
+++ b/P4/SEO_ANALYSIS.xlsx
@@ -7,14 +7,14 @@
     <workbookView windowWidth="22488" windowHeight="9335"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="SEO ANALYSIS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
   <si>
     <t>Category</t>
   </si>
@@ -79,24 +79,6 @@
     <t>Create a meta description for the contact page</t>
   </si>
   <si>
-    <t>Use alternative text for images</t>
-  </si>
-  <si>
-    <t>Alt text (text that describes an image) improves accessibility for people who can't see images on web pages, including users who use screen readers or have low-bandwidth connections.</t>
-  </si>
-  <si>
-    <t>https://support.google.com/webmasters/answer/114016?hl=en</t>
-  </si>
-  <si>
-    <t>Is the image's alternative useful?</t>
-  </si>
-  <si>
-    <t>When choosing alt text, focus on creating useful, information-rich content that uses keywords appropriately and is in context of the content of the page.</t>
-  </si>
-  <si>
-    <t>Change the alternate text and use a text which is describing the images.</t>
-  </si>
-  <si>
     <t>Use of headings tag</t>
   </si>
   <si>
@@ -119,13 +101,13 @@
     <t>Reduce the weight of the images using a optimizer like the google app squoosh.app</t>
   </si>
   <si>
+    <t>https://developers.google.com/web/fundamentals/performance/optimizing-content-efficiency/image-optimization</t>
+  </si>
+  <si>
     <t>Images format</t>
   </si>
   <si>
     <t>The images format can be optimized and format with a better compression can be used. We recommend converting them to webP format.</t>
-  </si>
-  <si>
-    <t>https://developers.google.com/web/fundamentals/performance/optimizing-content-efficiency/image-optimization</t>
   </si>
   <si>
     <t>Images size</t>
@@ -146,7 +128,101 @@
     <t>https://developers.google.com/web/fundamentals/performance/optimizing-content-efficiency/optimize-encoding-and-transfer</t>
   </si>
   <si>
+    <t>Avoid to delay the first paint of the webpage</t>
+  </si>
+  <si>
+    <t>JS should be called used the async or defer attribute,  so it will not delay the first paint of the website.</t>
+  </si>
+  <si>
+    <t>Try to async or defer the JS loading.</t>
+  </si>
+  <si>
+    <t>/web.dev/render-blocking-resources/</t>
+  </si>
+  <si>
+    <t>Cloaking</t>
+  </si>
+  <si>
+    <t>Hiding text for user and showing for crawlers is a black hat technique not recommended</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove the divs with the class "keyword" which are white on white </t>
+  </si>
+  <si>
+    <t>https://support.google.com/webmasters/answer/66355?hl=en</t>
+  </si>
+  <si>
+    <t>Page is indexable</t>
+  </si>
+  <si>
+    <t>Search engines can only show pages in their search results if those pages don't explicitly block indexing by search engine crawlers</t>
+  </si>
+  <si>
+    <t>https://web.dev/is-crawable/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO </t>
+  </si>
+  <si>
+    <t>Page is responding a 200OK</t>
+  </si>
+  <si>
+    <t>A webpage in order to be crawled and indexed should respond a 2xx HTTP Status Code</t>
+  </si>
+  <si>
+    <t>https://web.dev/http-status-code/</t>
+  </si>
+  <si>
+    <t>Internal Link</t>
+  </si>
+  <si>
+    <t>Internal links are importa and the anchor text should be usefulf, clear and relevant.</t>
+  </si>
+  <si>
+    <t>Change the anchor text in the menu for contact page. 
+Change the anchor text after the form from "other page" to "home page"</t>
+  </si>
+  <si>
+    <t>SEO/ACCESSIBILITY</t>
+  </si>
+  <si>
+    <t>Text instead of images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t embed important text inside images: Avoid embedding text in images, especially important text elements like page headings and menu items, because not all users can access them (and page translation tools won't work on images). To ensure maximum accessibility of your content, keep text in HTML, provide alt text for images. </t>
+  </si>
+  <si>
+    <t>Replace the images which contains only text  with a plain text</t>
+  </si>
+  <si>
+    <t>https://support.google.com/webmasters/answer/114016?hl=en</t>
+  </si>
+  <si>
     <t>ACCESSIBILITY</t>
+  </si>
+  <si>
+    <t>Label for accessibility</t>
+  </si>
+  <si>
+    <t>Include the form element inside the label tag</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/WAI/WCAG21/quickref/?showtechniques=143%2C246#headings-and-labels</t>
+  </si>
+  <si>
+    <t>Use alternative text for images</t>
+  </si>
+  <si>
+    <t>Alt text (text that describes an image) improves accessibility for people who can't see images on web pages, including users who use screen readers or have low-bandwidth connections.</t>
+  </si>
+  <si>
+    <t>Is the image's alternative text descriptive?</t>
+  </si>
+  <si>
+    <t>When choosing alt text, focus on creating useful, information-rich content that uses keywords appropriately and is in context of the content of the page.</t>
+  </si>
+  <si>
+    <t>Change the alternate text and use a text which is describing the images.</t>
   </si>
   <si>
     <t xml:space="preserve">Has the &lt;html&gt; a [lang] attribute </t>
@@ -161,68 +237,49 @@
     <t xml:space="preserve"> &lt;html&gt; element[lang] attribute is a valid code?</t>
   </si>
   <si>
-    <t>Setting the attribute lang="en"</t>
+    <t>A valid attribute for the html element lang is required by screen reader in order to correctly pronounce the text of the page.</t>
   </si>
   <si>
-    <t>Avoid to delay the first paint of the webpage</t>
-  </si>
-  <si>
-    <t>JS should be called used the async or defer attribute,  so it will not delay the first paint of the website.</t>
-  </si>
-  <si>
-    <t>SEO/ACCESSIBILITY</t>
-  </si>
-  <si>
-    <t>Text instead of images</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Don’t embed important text inside images: Avoid embedding text in images, especially important text elements like page headings and menu items, because not all users can access them (and page translation tools won't work on images). To ensure maximum accessibility of your content, keep text in HTML, provide alt text for images. </t>
-  </si>
-  <si>
-    <t>Replace the images which contains only text  with a plain text</t>
-  </si>
-  <si>
-    <t>Cloaking</t>
-  </si>
-  <si>
-    <t>Hiding text for user and showing for crawlers is a black hat technique not recommended</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove the divs with the class "keyword" which are white on white </t>
-  </si>
-  <si>
-    <t>https://support.google.com/webmasters/answer/66355?hl=en</t>
-  </si>
-  <si>
-    <t>Pages are responding a 200 OK</t>
-  </si>
-  <si>
-    <t>Links have descriptive text</t>
-  </si>
-  <si>
-    <t>Page is indexable</t>
-  </si>
-  <si>
-    <t>Use legible font size</t>
+    <t>Setting the attribute lang="en" instead of "default"</t>
   </si>
   <si>
     <t>Buttons have an accessible name</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">When a button doesn't have an accessible name, screen readers and other assistive technologies announce it as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>, which provides no information to users about what the button does.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://web.dev/button-name/</t>
+  </si>
+  <si>
     <t xml:space="preserve">User-scalable="no" in meta viewport </t>
   </si>
   <si>
-    <t>Maximum scale &gt; 5</t>
+    <t>Adding a `&lt;meta name="viewport"&gt;` tag is recommended in order to optimize a website for mobile devices</t>
   </si>
   <si>
-    <t>Internal Link</t>
-  </si>
-  <si>
-    <t>Internal links are importa and the anchor text should be usefulf, clear and relevant.</t>
-  </si>
-  <si>
-    <t>Change the anchor text in the menu for contact page. 
-Change the anchor text after the form from "other page" to "home page"</t>
+    <t>https://web.dev/viewport/</t>
   </si>
 </sst>
 </file>
@@ -230,12 +287,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,14 +341,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,6 +377,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -327,17 +410,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -350,8 +425,15 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -372,25 +454,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -404,11 +469,16 @@
     </font>
     <font>
       <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="34">
@@ -426,7 +496,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,7 +658,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,163 +670,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -644,24 +714,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -677,17 +729,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -709,24 +766,37 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -738,134 +808,134 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -881,6 +951,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1201,12 +1283,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:XFD25"/>
+  <dimension ref="A1:XFD23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="$A15:$XFD15"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -17693,58 +17775,63 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" ht="62.4" spans="2:6">
+    <row r="6" ht="62.4" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="7" ht="62.4" spans="2:6">
+    <row r="7" ht="46.8" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
+      <c r="D7" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>23</v>
+      <c r="F7" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="8" ht="62.4" spans="1:6">
+    <row r="8" ht="46.8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="D8" s="6"/>
       <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="F8" s="7"/>
     </row>
-    <row r="9" ht="46.8" spans="1:5">
+    <row r="9" ht="46.8" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -17754,27 +17841,29 @@
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="F9" s="8"/>
     </row>
-    <row r="10" ht="46.8" spans="1:6">
+    <row r="10" ht="43.2" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -17788,220 +17877,243 @@
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F11" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="12" ht="43.2" spans="1:6">
+    <row r="12" ht="31.2" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>42</v>
+      <c r="F12" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="13" ht="31.2" spans="1:6">
+    <row r="13" ht="46.8" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>45</v>
+      <c r="D13" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="14" ht="31.2" spans="1:5">
+    <row r="14" ht="31.2" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>12</v>
+      <c r="D14" s="9" t="s">
+        <v>50</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>48</v>
+      <c r="F14" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="15" ht="46.8" spans="1:4">
+    <row r="15" ht="62.4" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" ht="109.2" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="17" ht="31.2" spans="1:6">
+    <row r="17" ht="46.8" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>56</v>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>58</v>
+      <c r="F17" s="9" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" ht="62.4" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" ht="62.4" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" ht="31.2" spans="1:6">
+      <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" ht="46.8" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" ht="62.4" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D22" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" ht="46.8" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2" t="s">
-        <v>43</v>
+      <c r="D23" s="9" t="s">
+        <v>79</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" ht="62.4" spans="1:5">
-      <c r="A25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>68</v>
+      <c r="F23" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="F7:F9"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://support.google.com/webmasters/answer/35624?hl=en" tooltip="https://support.google.com/webmasters/answer/35624?hl=en"/>
     <hyperlink ref="F5" r:id="rId1" display="https://support.google.com/webmasters/answer/35624?hl=en"/>
-    <hyperlink ref="F6" r:id="rId2" display="https://support.google.com/webmasters/answer/114016?hl=en"/>
-    <hyperlink ref="F7" r:id="rId2" display="https://support.google.com/webmasters/answer/114016?hl=en"/>
-    <hyperlink ref="F16" r:id="rId2" display="https://support.google.com/webmasters/answer/114016?hl=en"/>
+    <hyperlink ref="F18" r:id="rId2" display="https://support.google.com/webmasters/answer/114016?hl=en"/>
+    <hyperlink ref="F19" r:id="rId2" display="https://support.google.com/webmasters/answer/114016?hl=en"/>
+    <hyperlink ref="F16" r:id="rId2" display="https://support.google.com/webmasters/answer/114016?hl=en" tooltip="https://support.google.com/webmasters/answer/114016?hl=en"/>
     <hyperlink ref="F2" r:id="rId1" display="https://support.google.com/webmasters/answer/35624?hl=en"/>
     <hyperlink ref="F4" r:id="rId3" display="https://webmasters.googleblog.com/2009/09/google-does-not-use-keywords-meta-tag.html"/>
-    <hyperlink ref="F12" r:id="rId4" display="https://developers.google.com/web/fundamentals/performance/optimizing-content-efficiency/optimize-encoding-and-transfer"/>
-    <hyperlink ref="F17" r:id="rId5" display="https://support.google.com/webmasters/answer/66355?hl=en"/>
+    <hyperlink ref="F10" r:id="rId4" display="https://developers.google.com/web/fundamentals/performance/optimizing-content-efficiency/optimize-encoding-and-transfer" tooltip="https://developers.google.com/web/fundamentals/performance/optimizing-content-efficiency/optimize-encoding-and-transfer"/>
+    <hyperlink ref="F12" r:id="rId5" display="https://support.google.com/webmasters/answer/66355?hl=en" tooltip="https://support.google.com/webmasters/answer/66355?hl=en"/>
+    <hyperlink ref="F6" r:id="rId6" display="https://support.google.com/webmasters/answer/7451184?hl=en"/>
+    <hyperlink ref="F7" r:id="rId7" display="https://developers.google.com/web/fundamentals/performance/optimizing-content-efficiency/image-optimization"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>